<commit_message>
Update storage location import to include a hierarchy
</commit_message>
<xml_diff>
--- a/museum/rwahsLocationHistoryMapping.xlsx
+++ b/museum/rwahsLocationHistoryMapping.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="335">
   <si>
     <t>Rule type</t>
   </si>
@@ -227,6 +227,9 @@
     <t>{"skipIfBlank":1}</t>
   </si>
   <si>
+    <t>A1992.95</t>
+  </si>
+  <si>
     <t>adminDonor</t>
   </si>
   <si>
@@ -242,7 +245,7 @@
     <t>Location</t>
   </si>
   <si>
-    <t>ca_movements.Location</t>
+    <t>mapped in topLevelLocation</t>
   </si>
   <si>
     <t>LocationDate</t>
@@ -261,6 +264,9 @@
   </si>
   <si>
     <t>ca_movements.PrimaryKey_Object_Table</t>
+  </si>
+  <si>
+    <t>not necessary to import</t>
   </si>
   <si>
     <t>o_Accession_Full_ID</t>
@@ -294,20 +300,35 @@
     <t>ca_storage_locations</t>
   </si>
   <si>
+    <t>childStorageLocation</t>
+  </si>
+  <si>
     <t>storageLocationSplitter</t>
   </si>
   <si>
     <t>{
-    "storageLocationType": "room",
+    "storageLocationType": "^childType",
     "relationshipType": "related",
+    "attributes":{
+        "idno": "%",
+        "is_enabled": true,
+        "status": "completed"
+    },
     "matchOn": [
         "label"
+    ],
+    "parents": [
+        {
+            "name": "^topLevelLocation",
+            "type": "room",
+            "idno": "%",
+            "attributes":{
+                "is_enabled": true
+            }
+        }
     ]
 }
 </t>
-  </si>
-  <si>
-    <t>childStorageLocation</t>
   </si>
   <si>
     <t>childType</t>
@@ -2130,9 +2151,11 @@
       <c r="K14" s="15"/>
       <c r="L14" s="31"/>
       <c r="M14" s="32"/>
-      <c r="N14" s="33"/>
+      <c r="N14" s="33" t="s">
+        <v>68</v>
+      </c>
       <c r="O14" s="33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P14" s="34"/>
       <c r="Q14" s="34"/>
@@ -2156,10 +2179,10 @@
         <v>64</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D15" s="29"/>
       <c r="E15" s="27" t="s">
@@ -2173,9 +2196,11 @@
       <c r="K15" s="15"/>
       <c r="L15" s="31"/>
       <c r="M15" s="32"/>
-      <c r="N15" s="33"/>
+      <c r="N15" s="33" t="s">
+        <v>68</v>
+      </c>
       <c r="O15" s="33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P15" s="34"/>
       <c r="Q15" s="34"/>
@@ -2196,14 +2221,12 @@
     </row>
     <row r="16">
       <c r="A16" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="7" t="s">
         <v>73</v>
       </c>
+      <c r="C16" s="7"/>
       <c r="D16" s="29"/>
       <c r="E16" s="27" t="s">
         <v>67</v>
@@ -2213,7 +2236,9 @@
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
+      <c r="K16" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="L16" s="31"/>
       <c r="M16" s="32" t="str">
         <f t="shared" ref="M16:M18" si="1">validateJson(E16, G16)</f>
@@ -2221,7 +2246,7 @@
       </c>
       <c r="N16" s="33"/>
       <c r="O16" s="33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P16" s="34" t="str">
         <f>VLOOKUP($B16,sampleDataObjects,P$1,false)</f>
@@ -2249,15 +2274,15 @@
       </c>
       <c r="V16" s="37" t="str">
         <f t="shared" ref="V16:V20" si="2">C16</f>
-        <v>ca_movements.Location</v>
+        <v/>
       </c>
       <c r="W16" s="34" t="str">
         <f t="shared" ref="W16:W20" si="3">iferror(left(V16, find(".", V16) -1),"")</f>
-        <v>ca_movements</v>
+        <v/>
       </c>
       <c r="X16" s="34" t="str">
         <f t="shared" ref="X16:X20" si="4">if(len(W16) &gt; 0,iferror(right(V16, len(V16) - len(W16) -1),""),"")</f>
-        <v>Location</v>
+        <v/>
       </c>
       <c r="Y16" s="37" t="str">
         <f t="shared" ref="Y16:Y20" si="5">B16</f>
@@ -2297,10 +2322,10 @@
         <v>64</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D17" s="29"/>
       <c r="E17" s="27" t="s">
@@ -2317,9 +2342,11 @@
         <f t="shared" si="1"/>
         <v>TRUE</v>
       </c>
-      <c r="N17" s="33"/>
+      <c r="N17" s="33" t="s">
+        <v>68</v>
+      </c>
       <c r="O17" s="33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P17" s="34" t="str">
         <f>VLOOKUP($B17,sampleDataObjects,P$1,false)</f>
@@ -2385,10 +2412,10 @@
         <v>64</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D18" s="29"/>
       <c r="E18" s="27" t="s">
@@ -2407,7 +2434,7 @@
       </c>
       <c r="N18" s="33"/>
       <c r="O18" s="33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P18" s="34" t="str">
         <f>VLOOKUP($B18,sampleDataObjects,P$1,false)</f>
@@ -2470,13 +2497,13 @@
     </row>
     <row r="19">
       <c r="A19" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D19" s="38"/>
       <c r="E19" s="27" t="s">
@@ -2487,12 +2514,14 @@
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
-      <c r="K19" s="7"/>
+      <c r="K19" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="L19" s="31"/>
       <c r="M19" s="32"/>
       <c r="N19" s="33"/>
       <c r="O19" s="33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P19" s="34" t="str">
         <f>VLOOKUP($B19,sampleDataObjects,P$1,false)</f>
@@ -2544,20 +2573,20 @@
         <v>64</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D20" s="29"/>
       <c r="E20" s="27" t="s">
         <v>67</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
@@ -2568,9 +2597,11 @@
         <f>validateJson(E20, G20)</f>
         <v>TRUE</v>
       </c>
-      <c r="N20" s="33"/>
+      <c r="N20" s="33" t="s">
+        <v>68</v>
+      </c>
       <c r="O20" s="33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P20" s="34" t="str">
         <f>VLOOKUP($B20,sampleDataObjects,P$1,false)</f>
@@ -2633,13 +2664,13 @@
     </row>
     <row r="21">
       <c r="A21" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D21" s="29"/>
       <c r="E21" s="27" t="s">
@@ -2652,9 +2683,11 @@
       <c r="K21" s="7"/>
       <c r="L21" s="31"/>
       <c r="M21" s="32"/>
-      <c r="N21" s="33"/>
+      <c r="N21" s="33" t="s">
+        <v>68</v>
+      </c>
       <c r="O21" s="33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P21" s="34"/>
       <c r="Q21" s="34"/>
@@ -2675,24 +2708,20 @@
     </row>
     <row r="22">
       <c r="A22" s="27" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D22" s="29"/>
       <c r="E22" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G22" s="30" t="s">
-        <v>89</v>
-      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="30"/>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
@@ -2701,7 +2730,7 @@
       <c r="M22" s="32"/>
       <c r="N22" s="33"/>
       <c r="O22" s="33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P22" s="34" t="str">
         <f>VLOOKUP($B22,sampleDataObjects,P$1,false)</f>
@@ -2761,19 +2790,25 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="27"/>
+      <c r="A23" s="27" t="s">
+        <v>64</v>
+      </c>
       <c r="B23" s="7" t="s">
         <v>90</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D23" s="29"/>
       <c r="E23" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="15"/>
-      <c r="G23" s="36"/>
+      <c r="F23" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" s="30" t="s">
+        <v>92</v>
+      </c>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="15"/>
@@ -2782,7 +2817,7 @@
       <c r="M23" s="32"/>
       <c r="N23" s="33"/>
       <c r="O23" s="33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P23" s="34" t="str">
         <f>VLOOKUP($B23,sampleDataObjects,P$1,false)</f>
@@ -2832,12 +2867,14 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="27"/>
+      <c r="A24" s="27" t="s">
+        <v>72</v>
+      </c>
       <c r="B24" s="28" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D24" s="38"/>
       <c r="E24" s="27" t="s">
@@ -2856,7 +2893,7 @@
       </c>
       <c r="N24" s="33"/>
       <c r="O24" s="33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P24" s="34" t="str">
         <f>VLOOKUP($B24,sampleDataObjects,P$1,false)</f>
@@ -2940,7 +2977,7 @@
       </c>
       <c r="N25" s="33"/>
       <c r="O25" s="33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P25" s="34" t="str">
         <f>VLOOKUP($B25,sampleDataObjects,P$1,false)</f>
@@ -3019,7 +3056,7 @@
       <c r="M26" s="32"/>
       <c r="N26" s="33"/>
       <c r="O26" s="33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P26" s="34" t="str">
         <f>VLOOKUP($B26,sampleDataObjects,P$1,false)</f>
@@ -3086,7 +3123,7 @@
       <c r="M27" s="32"/>
       <c r="N27" s="33"/>
       <c r="O27" s="33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P27" s="34" t="str">
         <f>VLOOKUP($B27,sampleDataObjects,P$1,false)</f>
@@ -3153,7 +3190,7 @@
       <c r="M28" s="32"/>
       <c r="N28" s="33"/>
       <c r="O28" s="33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P28" s="34" t="str">
         <f>VLOOKUP($B28,sampleDataObjects,P$1,false)</f>
@@ -3346,7 +3383,7 @@
         <v/>
       </c>
       <c r="Z30" s="33" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AA30" s="34"/>
       <c r="AB30" s="34"/>
@@ -3388,7 +3425,7 @@
       <c r="M31" s="32"/>
       <c r="N31" s="33"/>
       <c r="O31" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P31" s="34" t="str">
         <f>VLOOKUP($B31,sampleDataObjects,P$1,false)</f>
@@ -3416,7 +3453,7 @@
         <v/>
       </c>
       <c r="Z31" s="33" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AA31" s="34"/>
       <c r="AB31" s="34"/>
@@ -3460,7 +3497,7 @@
       </c>
       <c r="N32" s="33"/>
       <c r="O32" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P32" s="34" t="str">
         <f>VLOOKUP($B32,sampleDataObjects,P$1,false)</f>
@@ -3503,7 +3540,7 @@
         <v/>
       </c>
       <c r="Z32" s="33" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AA32" s="34"/>
       <c r="AB32" s="34" t="str">
@@ -3551,7 +3588,7 @@
       </c>
       <c r="N33" s="33"/>
       <c r="O33" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P33" s="34" t="str">
         <f>VLOOKUP($B33,sampleDataObjects,P$1,false)</f>
@@ -3594,7 +3631,7 @@
         <v/>
       </c>
       <c r="Z33" s="33" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AA33" s="34"/>
       <c r="AB33" s="34" t="str">
@@ -3642,7 +3679,7 @@
       </c>
       <c r="N34" s="33"/>
       <c r="O34" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P34" s="34" t="str">
         <f>VLOOKUP($B34,sampleDataObjects,P$1,false)</f>
@@ -3670,7 +3707,7 @@
         <v/>
       </c>
       <c r="Z34" s="33" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AA34" s="34"/>
       <c r="AB34" s="34"/>
@@ -3712,7 +3749,7 @@
       </c>
       <c r="N35" s="33"/>
       <c r="O35" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P35" s="34" t="str">
         <f>VLOOKUP($B35,sampleDataObjects,P$1,false)</f>
@@ -3755,7 +3792,7 @@
         <v/>
       </c>
       <c r="Z35" s="33" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AA35" s="34"/>
       <c r="AB35" s="34" t="str">
@@ -3803,7 +3840,7 @@
       </c>
       <c r="N36" s="33"/>
       <c r="O36" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P36" s="34" t="str">
         <f>VLOOKUP($B36,sampleDataObjects,P$1,false)</f>
@@ -3831,7 +3868,7 @@
         <v/>
       </c>
       <c r="Z36" s="33" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AA36" s="34"/>
       <c r="AB36" s="34"/>
@@ -3873,7 +3910,7 @@
       </c>
       <c r="N37" s="33"/>
       <c r="O37" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P37" s="34" t="str">
         <f>VLOOKUP($B37,sampleDataObjects,P$1,false)</f>
@@ -3916,7 +3953,7 @@
         <v/>
       </c>
       <c r="Z37" s="33" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="AA37" s="34"/>
       <c r="AB37" s="34" t="str">
@@ -3964,7 +4001,7 @@
       </c>
       <c r="N38" s="33"/>
       <c r="O38" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P38" s="34" t="str">
         <f>VLOOKUP($B38,sampleDataObjects,P$1,false)</f>
@@ -3992,7 +4029,7 @@
         <v/>
       </c>
       <c r="Z38" s="33" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AA38" s="34"/>
       <c r="AB38" s="34"/>
@@ -4344,7 +4381,7 @@
       </c>
       <c r="N44" s="33"/>
       <c r="O44" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P44" s="34" t="str">
         <f>VLOOKUP($B44,sampleDataObjects,P$1,false)</f>
@@ -4390,7 +4427,7 @@
         <v>20</v>
       </c>
       <c r="AA44" s="33" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="AB44" s="34" t="str">
         <f>VLOOKUP($B44,sampleDataObjects,AB$1,false)</f>
@@ -4437,7 +4474,7 @@
       </c>
       <c r="N45" s="33"/>
       <c r="O45" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P45" s="34" t="str">
         <f>VLOOKUP($B45,sampleDataObjects,P$1,false)</f>
@@ -4483,7 +4520,7 @@
         <v>20</v>
       </c>
       <c r="AA45" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AB45" s="34" t="str">
         <f>VLOOKUP($B45,sampleDataObjects,AB$1,false)</f>
@@ -4520,7 +4557,7 @@
       </c>
       <c r="N46" s="33"/>
       <c r="O46" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P46" s="34" t="str">
         <f>VLOOKUP($B46,sampleDataObjects,P$1,false)</f>
@@ -4566,7 +4603,7 @@
         <v>20</v>
       </c>
       <c r="AA46" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AB46" s="34" t="str">
         <f>VLOOKUP($B46,sampleDataObjects,AB$1,false)</f>
@@ -4603,7 +4640,7 @@
       </c>
       <c r="N47" s="33"/>
       <c r="O47" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P47" s="34" t="str">
         <f>VLOOKUP($B47,sampleDataObjects,P$1,false)</f>
@@ -4649,7 +4686,7 @@
         <v>20</v>
       </c>
       <c r="AA47" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AB47" s="34" t="str">
         <f>VLOOKUP($B47,sampleDataObjects,AB$1,false)</f>
@@ -4686,7 +4723,7 @@
       </c>
       <c r="N48" s="33"/>
       <c r="O48" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P48" s="34" t="str">
         <f>VLOOKUP($B48,sampleDataObjects,P$1,false)</f>
@@ -4732,7 +4769,7 @@
         <v>20</v>
       </c>
       <c r="AA48" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AB48" s="34" t="str">
         <f>VLOOKUP($B48,sampleDataObjects,AB$1,false)</f>
@@ -4769,7 +4806,7 @@
       </c>
       <c r="N49" s="33"/>
       <c r="O49" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P49" s="34" t="str">
         <f>VLOOKUP($B49,sampleDataObjects,P$1,false)</f>
@@ -4815,7 +4852,7 @@
         <v>20</v>
       </c>
       <c r="AA49" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AB49" s="34" t="str">
         <f>VLOOKUP($B49,sampleDataObjects,AB$1,false)</f>
@@ -4852,7 +4889,7 @@
       </c>
       <c r="N50" s="33"/>
       <c r="O50" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P50" s="34" t="str">
         <f>VLOOKUP($B50,sampleDataObjects,P$1,false)</f>
@@ -4883,7 +4920,7 @@
         <v>20</v>
       </c>
       <c r="AA50" s="33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AB50" s="34"/>
       <c r="AC50" s="34"/>
@@ -4914,7 +4951,7 @@
       </c>
       <c r="N51" s="33"/>
       <c r="O51" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P51" s="34" t="str">
         <f>VLOOKUP($B51,sampleDataObjects,P$1,false)</f>
@@ -4945,7 +4982,7 @@
         <v>20</v>
       </c>
       <c r="AA51" s="33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AB51" s="34"/>
       <c r="AC51" s="34"/>
@@ -4976,7 +5013,7 @@
       </c>
       <c r="N52" s="33"/>
       <c r="O52" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P52" s="34" t="str">
         <f>VLOOKUP($B52,sampleDataObjects,P$1,false)</f>
@@ -5022,7 +5059,7 @@
         <v>20</v>
       </c>
       <c r="AA52" s="33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AB52" s="34" t="str">
         <f>VLOOKUP($B52,sampleDataObjects,AB$1,false)</f>
@@ -5059,7 +5096,7 @@
       </c>
       <c r="N53" s="33"/>
       <c r="O53" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P53" s="34" t="str">
         <f>VLOOKUP($B53,sampleDataObjects,P$1,false)</f>
@@ -5105,7 +5142,7 @@
         <v>20</v>
       </c>
       <c r="AA53" s="33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AB53" s="34" t="str">
         <f>VLOOKUP($B53,sampleDataObjects,AB$1,false)</f>
@@ -5142,7 +5179,7 @@
       </c>
       <c r="N54" s="33"/>
       <c r="O54" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P54" s="34" t="str">
         <f>VLOOKUP($B54,sampleDataObjects,P$1,false)</f>
@@ -5188,7 +5225,7 @@
         <v>20</v>
       </c>
       <c r="AA54" s="33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AB54" s="34" t="str">
         <f>VLOOKUP($B54,sampleDataObjects,AB$1,false)</f>
@@ -5225,7 +5262,7 @@
       </c>
       <c r="N55" s="33"/>
       <c r="O55" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P55" s="34" t="str">
         <f>VLOOKUP($B55,sampleDataObjects,P$1,false)</f>
@@ -5271,7 +5308,7 @@
         <v>20</v>
       </c>
       <c r="AA55" s="33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AB55" s="34" t="str">
         <f>VLOOKUP($B55,sampleDataObjects,AB$1,false)</f>
@@ -5308,7 +5345,7 @@
       </c>
       <c r="N56" s="33"/>
       <c r="O56" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P56" s="34" t="str">
         <f>VLOOKUP($B56,sampleDataObjects,P$1,false)</f>
@@ -5354,7 +5391,7 @@
         <v>20</v>
       </c>
       <c r="AA56" s="33" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AB56" s="34" t="str">
         <f>VLOOKUP($B56,sampleDataObjects,AB$1,false)</f>
@@ -5391,7 +5428,7 @@
       </c>
       <c r="N57" s="33"/>
       <c r="O57" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P57" s="34" t="str">
         <f>VLOOKUP($B57,sampleDataObjects,P$1,false)</f>
@@ -5434,7 +5471,7 @@
         <v/>
       </c>
       <c r="Z57" s="33" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AA57" s="34"/>
       <c r="AB57" s="34" t="str">
@@ -5472,7 +5509,7 @@
       </c>
       <c r="N58" s="33"/>
       <c r="O58" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P58" s="34" t="str">
         <f>VLOOKUP($B58,sampleDataObjects,P$1,false)</f>
@@ -5515,7 +5552,7 @@
         <v/>
       </c>
       <c r="Z58" s="33" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AA58" s="34"/>
       <c r="AB58" s="34" t="str">
@@ -5550,7 +5587,7 @@
       <c r="M59" s="32"/>
       <c r="N59" s="33"/>
       <c r="O59" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P59" s="34" t="str">
         <f>VLOOKUP($B59,sampleDataObjects,P$1,false)</f>
@@ -5578,7 +5615,7 @@
         <v/>
       </c>
       <c r="Z59" s="33" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AA59" s="34"/>
       <c r="AB59" s="34"/>
@@ -6765,7 +6802,7 @@
       </c>
       <c r="N75" s="33"/>
       <c r="O75" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P75" s="34" t="str">
         <f>VLOOKUP($B75,sampleDataObjects,P$1,false)</f>
@@ -6811,7 +6848,7 @@
         <v>20</v>
       </c>
       <c r="AA75" s="33" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AB75" s="34" t="str">
         <f>VLOOKUP($B75,sampleDataObjects,AB$1,false)</f>
@@ -6858,7 +6895,7 @@
       </c>
       <c r="N76" s="33"/>
       <c r="O76" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P76" s="34" t="str">
         <f>VLOOKUP($B76,sampleDataObjects,P$1,false)</f>
@@ -7250,7 +7287,7 @@
       </c>
       <c r="N81" s="33"/>
       <c r="O81" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P81" s="34" t="str">
         <f>VLOOKUP($B81,sampleDataObjects,P$1,false)</f>
@@ -7339,7 +7376,7 @@
       </c>
       <c r="N82" s="33"/>
       <c r="O82" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P82" s="34" t="str">
         <f>VLOOKUP($B82,sampleDataObjects,P$1,false)</f>
@@ -7462,7 +7499,7 @@
         <v>20</v>
       </c>
       <c r="AA83" s="33" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AB83" s="34" t="str">
         <f>VLOOKUP($B83,sampleDataObjects,AB$1,false)</f>
@@ -13850,7 +13887,7 @@
     </row>
     <row r="2">
       <c r="A2" s="50" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B2" s="50" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IMPORTRANGE(""1lzo91LeaCrl2WIh-P0JoIdjtaSyV-lug3mWSMAt2N_s"", ""dataReport!A1:K400"")"),"#REF!")</f>
@@ -19890,19 +19927,19 @@
         <v>3</v>
       </c>
       <c r="K1" s="50" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L1" s="50" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M1" s="50" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="N1" s="50" t="s">
         <v>20</v>
       </c>
       <c r="O1" s="50" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2">
@@ -20505,14 +20542,14 @@
       </c>
       <c r="I101" s="51"/>
       <c r="J101" s="50" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="K101" t="str">
         <f>vlookup(C101,Mapping!$B$14:$C$127,2,false)</f>
         <v>#N/A</v>
       </c>
       <c r="M101" s="50" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="102">
@@ -20525,7 +20562,7 @@
         <v>#N/A</v>
       </c>
       <c r="M102" s="50" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N102" s="50"/>
     </row>
@@ -20539,7 +20576,7 @@
         <v>#N/A</v>
       </c>
       <c r="M103" s="50" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="104">
@@ -20552,7 +20589,7 @@
         <v>#N/A</v>
       </c>
       <c r="M104" s="50" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="105">
@@ -20565,7 +20602,7 @@
         <v>#N/A</v>
       </c>
       <c r="M105" s="50" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="106">
@@ -20578,7 +20615,7 @@
         <v>#N/A</v>
       </c>
       <c r="M106" s="50" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="107">
@@ -20587,7 +20624,7 @@
       </c>
       <c r="I107" s="51"/>
       <c r="J107" s="50" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="K107" t="str">
         <f>vlookup(C107,Mapping!$B$14:$C$127,2,false)</f>
@@ -20607,7 +20644,7 @@
         <v>#N/A</v>
       </c>
       <c r="M108" s="50" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="109">
@@ -20623,7 +20660,7 @@
         <v>0.0</v>
       </c>
       <c r="M109" s="50" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="110">
@@ -30427,10 +30464,10 @@
     </row>
     <row r="3">
       <c r="A3" s="52" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C3" s="54" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D3" s="53" t="str">
         <f t="shared" ref="D3:D7" si="1">"&lt;list code='" &amp; A3&amp;"' hierarchical='0' system='0' vocabulary='1'&gt;
@@ -30443,10 +30480,10 @@
     </row>
     <row r="4">
       <c r="A4" s="52" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D4" s="53" t="str">
         <f t="shared" si="1"/>
@@ -30457,10 +30494,10 @@
     </row>
     <row r="5">
       <c r="A5" s="52" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D5" s="53" t="str">
         <f t="shared" si="1"/>
@@ -30471,10 +30508,10 @@
     </row>
     <row r="6">
       <c r="A6" s="52" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D6" s="53" t="str">
         <f t="shared" si="1"/>
@@ -30485,10 +30522,10 @@
     </row>
     <row r="7">
       <c r="A7" s="52" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D7" s="53" t="str">
         <f t="shared" si="1"/>
@@ -30499,7 +30536,7 @@
     </row>
     <row r="8">
       <c r="A8" s="52" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9">
@@ -33513,12 +33550,12 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="50" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="50" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B2" t="str">
         <f>"&lt;screen idno='"&amp;lower(A2)&amp;"' default='1'&gt;&lt;labels&gt;&lt;label locale='en_AU'&gt;&lt;name&gt;"&amp;A2&amp;"&lt;/name&gt;&lt;/label&gt;&lt;/labels&gt;&lt;typeRestrictions&gt;&lt;restriction type='museum_childhood'/&gt;&lt;/typeRestrictions&gt;&lt;bundlePlacements&gt;&lt;/bundlePlacements&gt;&lt;/screen&gt;"</f>
@@ -33527,7 +33564,7 @@
     </row>
     <row r="3">
       <c r="A3" s="50" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" ref="B3:B7" si="1">"&lt;screen idno='"&amp;lower(A3)&amp;"' default='0'&gt;&lt;labels&gt;&lt;label locale='en_AU'&gt;&lt;name&gt;"&amp;A3&amp;"&lt;/name&gt;&lt;/label&gt;&lt;/labels&gt;&lt;typeRestrictions&gt;&lt;restriction type='museum_childhood'/&gt;&lt;/typeRestrictions&gt;&lt;bundlePlacements&gt;&lt;/bundlePlacements&gt;&lt;/screen&gt;"</f>
@@ -33589,28 +33626,28 @@
         <v>64</v>
       </c>
       <c r="B1" s="55" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C1" s="56" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D1" s="55" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E1" s="55" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F1" s="55" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G1" s="56" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H1" s="57" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I1" s="57" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J1" s="58" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("filter($F:$F,NOT(REGEXMATCH($F:$F,""_x_"")))"),"ca_collections")</f>
@@ -33621,7 +33658,7 @@
         <v>ca_collections_x_collections</v>
       </c>
       <c r="L1" s="57" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="M1" s="58"/>
       <c r="N1" s="58"/>
@@ -33640,40 +33677,40 @@
     </row>
     <row r="2">
       <c r="A2" s="55" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B2" s="55" t="s">
         <v>57</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D2" s="55" t="s">
         <v>60</v>
       </c>
       <c r="E2" s="55" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F2" s="55" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G2" s="56" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H2" s="57" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I2" s="57" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J2" s="58" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="K2" s="58" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="L2" s="57" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="M2" s="58"/>
       <c r="N2" s="58"/>
@@ -33696,32 +33733,32 @@
       </c>
       <c r="B3" s="59"/>
       <c r="C3" s="56" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D3" s="59"/>
       <c r="E3" s="55" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F3" s="55" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G3" s="56" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H3" s="57" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I3" s="57" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="J3" s="58" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K3" s="58" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="L3" s="57" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="M3" s="58"/>
       <c r="N3" s="58"/>
@@ -33740,7 +33777,7 @@
     </row>
     <row r="4">
       <c r="A4" s="55" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B4" s="59"/>
       <c r="C4" s="56" t="s">
@@ -33748,28 +33785,28 @@
       </c>
       <c r="D4" s="59"/>
       <c r="E4" s="55" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F4" s="55" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G4" s="56" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H4" s="57" t="s">
         <v>20</v>
       </c>
       <c r="I4" s="57" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="J4" s="58" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K4" s="58" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="L4" s="57" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="M4" s="58"/>
       <c r="N4" s="58"/>
@@ -33788,36 +33825,36 @@
     </row>
     <row r="5">
       <c r="A5" s="55" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B5" s="59"/>
       <c r="C5" s="56" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D5" s="59"/>
       <c r="E5" s="55" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F5" s="55" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G5" s="56" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H5" s="57" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I5" s="57" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J5" s="58" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K5" s="58" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="L5" s="57" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="M5" s="58"/>
       <c r="N5" s="58"/>
@@ -33836,36 +33873,36 @@
     </row>
     <row r="6">
       <c r="A6" s="60" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B6" s="59"/>
       <c r="C6" s="56" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D6" s="59"/>
       <c r="E6" s="55" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F6" s="55" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G6" s="56" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H6" s="57" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="I6" s="57" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="J6" s="58" t="s">
         <v>43</v>
       </c>
       <c r="K6" s="58" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="L6" s="57" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="M6" s="58"/>
       <c r="N6" s="58"/>
@@ -33886,32 +33923,32 @@
       <c r="A7" s="59"/>
       <c r="B7" s="59"/>
       <c r="C7" s="56" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D7" s="59"/>
       <c r="E7" s="55" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F7" s="55" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G7" s="56" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H7" s="57" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I7" s="57" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="J7" s="58" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="K7" s="58" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="L7" s="57" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="M7" s="58"/>
       <c r="N7" s="58"/>
@@ -33932,32 +33969,32 @@
       <c r="A8" s="59"/>
       <c r="B8" s="59"/>
       <c r="C8" s="56" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D8" s="59"/>
       <c r="E8" s="60" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F8" s="55" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="G8" s="56" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="H8" s="57" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="I8" s="57" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="J8" s="58" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="K8" s="58" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="L8" s="57" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="M8" s="58"/>
       <c r="N8" s="58"/>
@@ -33978,30 +34015,30 @@
       <c r="A9" s="59"/>
       <c r="B9" s="59"/>
       <c r="C9" s="56" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D9" s="59"/>
       <c r="E9" s="60" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F9" s="55" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G9" s="56" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H9" s="57" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="I9" s="58"/>
       <c r="J9" s="58" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="K9" s="58" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="L9" s="57" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="M9" s="58"/>
       <c r="N9" s="58"/>
@@ -34022,30 +34059,30 @@
       <c r="A10" s="59"/>
       <c r="B10" s="59"/>
       <c r="C10" s="56" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D10" s="59"/>
       <c r="E10" s="60" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F10" s="55" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="G10" s="56" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H10" s="57" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="I10" s="58"/>
       <c r="J10" s="58" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="K10" s="58" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="L10" s="57" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="M10" s="58"/>
       <c r="N10" s="58"/>
@@ -34066,30 +34103,30 @@
       <c r="A11" s="59"/>
       <c r="B11" s="59"/>
       <c r="C11" s="56" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D11" s="59"/>
       <c r="E11" s="60" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="F11" s="55" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G11" s="56" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="H11" s="57" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I11" s="58"/>
       <c r="J11" s="58" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K11" s="58" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="L11" s="57" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="M11" s="58"/>
       <c r="N11" s="58"/>
@@ -34110,30 +34147,30 @@
       <c r="A12" s="59"/>
       <c r="B12" s="59"/>
       <c r="C12" s="56" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D12" s="59"/>
       <c r="E12" s="60" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F12" s="55" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G12" s="56" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="H12" s="57" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="I12" s="58"/>
       <c r="J12" s="58" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="K12" s="58" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="L12" s="57" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="M12" s="58"/>
       <c r="N12" s="58"/>
@@ -34154,30 +34191,30 @@
       <c r="A13" s="59"/>
       <c r="B13" s="59"/>
       <c r="C13" s="56" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D13" s="59"/>
       <c r="E13" s="60" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F13" s="55" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="G13" s="56" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H13" s="57" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="I13" s="58"/>
       <c r="J13" s="58" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="K13" s="58" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="L13" s="57" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="M13" s="58"/>
       <c r="N13" s="58"/>
@@ -34200,26 +34237,26 @@
       <c r="C14" s="59"/>
       <c r="D14" s="59"/>
       <c r="E14" s="60" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F14" s="55" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G14" s="56" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H14" s="57" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="I14" s="58"/>
       <c r="J14" s="58" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="K14" s="58" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="L14" s="57" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="M14" s="58"/>
       <c r="N14" s="58"/>
@@ -34243,23 +34280,23 @@
       <c r="D15" s="59"/>
       <c r="E15" s="59"/>
       <c r="F15" s="55" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G15" s="56" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="H15" s="57" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="I15" s="58"/>
       <c r="J15" s="58" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="K15" s="58" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="L15" s="57" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="M15" s="58"/>
       <c r="N15" s="58"/>
@@ -34283,23 +34320,23 @@
       <c r="D16" s="59"/>
       <c r="E16" s="59"/>
       <c r="F16" s="55" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="G16" s="56" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="H16" s="57" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="I16" s="58"/>
       <c r="J16" s="58" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="K16" s="58" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="L16" s="57" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="M16" s="58"/>
       <c r="N16" s="58"/>
@@ -34323,21 +34360,21 @@
       <c r="D17" s="59"/>
       <c r="E17" s="59"/>
       <c r="F17" s="60" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="G17" s="56" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="H17" s="57" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="I17" s="58"/>
       <c r="J17" s="58"/>
       <c r="K17" s="58" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L17" s="57" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="M17" s="58"/>
       <c r="N17" s="58"/>
@@ -34361,21 +34398,21 @@
       <c r="D18" s="59"/>
       <c r="E18" s="59"/>
       <c r="F18" s="60" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="G18" s="56" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="H18" s="57" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="I18" s="58"/>
       <c r="J18" s="58"/>
       <c r="K18" s="58" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="L18" s="57" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="M18" s="58"/>
       <c r="N18" s="58"/>
@@ -34399,21 +34436,21 @@
       <c r="D19" s="59"/>
       <c r="E19" s="59"/>
       <c r="F19" s="60" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="G19" s="56" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H19" s="57" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="I19" s="58"/>
       <c r="J19" s="58"/>
       <c r="K19" s="58" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="L19" s="57" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="M19" s="58"/>
       <c r="N19" s="58"/>
@@ -34437,21 +34474,21 @@
       <c r="D20" s="59"/>
       <c r="E20" s="59"/>
       <c r="F20" s="60" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="G20" s="56" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="H20" s="57" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="I20" s="58"/>
       <c r="J20" s="58"/>
       <c r="K20" s="58" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="L20" s="57" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="M20" s="58"/>
       <c r="N20" s="58"/>
@@ -34475,21 +34512,21 @@
       <c r="D21" s="59"/>
       <c r="E21" s="59"/>
       <c r="F21" s="60" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="G21" s="56" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="H21" s="57" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="I21" s="58"/>
       <c r="J21" s="58"/>
       <c r="K21" s="58" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="L21" s="57" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="M21" s="58"/>
       <c r="N21" s="58"/>
@@ -34513,21 +34550,21 @@
       <c r="D22" s="59"/>
       <c r="E22" s="59"/>
       <c r="F22" s="60" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G22" s="56" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="H22" s="57" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="I22" s="58"/>
       <c r="J22" s="58"/>
       <c r="K22" s="58" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="L22" s="57" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="M22" s="58"/>
       <c r="N22" s="58"/>
@@ -34551,21 +34588,21 @@
       <c r="D23" s="59"/>
       <c r="E23" s="59"/>
       <c r="F23" s="60" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="G23" s="56" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="H23" s="57" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="I23" s="58"/>
       <c r="J23" s="58"/>
       <c r="K23" s="58" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="L23" s="57" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="M23" s="58"/>
       <c r="N23" s="58"/>
@@ -34589,21 +34626,21 @@
       <c r="D24" s="59"/>
       <c r="E24" s="59"/>
       <c r="F24" s="60" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="G24" s="56" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="H24" s="57" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="I24" s="58"/>
       <c r="J24" s="58"/>
       <c r="K24" s="58" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="L24" s="57" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="M24" s="58"/>
       <c r="N24" s="58"/>
@@ -34627,21 +34664,21 @@
       <c r="D25" s="59"/>
       <c r="E25" s="59"/>
       <c r="F25" s="60" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="G25" s="56" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H25" s="57" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="I25" s="58"/>
       <c r="J25" s="58"/>
       <c r="K25" s="58" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="L25" s="57" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="M25" s="58"/>
       <c r="N25" s="58"/>
@@ -34665,21 +34702,21 @@
       <c r="D26" s="59"/>
       <c r="E26" s="59"/>
       <c r="F26" s="60" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="G26" s="56" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="H26" s="57" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="I26" s="58"/>
       <c r="J26" s="58"/>
       <c r="K26" s="58" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="L26" s="57" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="M26" s="58"/>
       <c r="N26" s="58"/>
@@ -34706,18 +34743,18 @@
         <v>43</v>
       </c>
       <c r="G27" s="56" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="H27" s="57" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="I27" s="58"/>
       <c r="J27" s="58"/>
       <c r="K27" s="58" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="L27" s="57" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="M27" s="58"/>
       <c r="N27" s="58"/>
@@ -34741,17 +34778,17 @@
       <c r="D28" s="59"/>
       <c r="E28" s="59"/>
       <c r="F28" s="60" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="G28" s="59"/>
       <c r="H28" s="58"/>
       <c r="I28" s="58"/>
       <c r="J28" s="58"/>
       <c r="K28" s="58" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="L28" s="57" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="M28" s="58"/>
       <c r="N28" s="58"/>
@@ -34775,17 +34812,17 @@
       <c r="D29" s="58"/>
       <c r="E29" s="58"/>
       <c r="F29" s="57" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="G29" s="58"/>
       <c r="H29" s="58"/>
       <c r="I29" s="58"/>
       <c r="J29" s="58"/>
       <c r="K29" s="58" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="L29" s="57" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="M29" s="58"/>
       <c r="N29" s="58"/>
@@ -34809,17 +34846,17 @@
       <c r="D30" s="58"/>
       <c r="E30" s="58"/>
       <c r="F30" s="57" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="G30" s="58"/>
       <c r="H30" s="58"/>
       <c r="I30" s="58"/>
       <c r="J30" s="58"/>
       <c r="K30" s="58" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="L30" s="57" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="M30" s="58"/>
       <c r="N30" s="58"/>
@@ -34843,17 +34880,17 @@
       <c r="D31" s="58"/>
       <c r="E31" s="58"/>
       <c r="F31" s="57" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="G31" s="58"/>
       <c r="H31" s="58"/>
       <c r="I31" s="58"/>
       <c r="J31" s="58"/>
       <c r="K31" s="58" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="L31" s="57" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="M31" s="58"/>
       <c r="N31" s="58"/>
@@ -34877,17 +34914,17 @@
       <c r="D32" s="58"/>
       <c r="E32" s="58"/>
       <c r="F32" s="57" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="G32" s="58"/>
       <c r="H32" s="58"/>
       <c r="I32" s="58"/>
       <c r="J32" s="58"/>
       <c r="K32" s="58" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="L32" s="57" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="M32" s="58"/>
       <c r="N32" s="58"/>
@@ -34911,17 +34948,17 @@
       <c r="D33" s="58"/>
       <c r="E33" s="58"/>
       <c r="F33" s="57" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="G33" s="58"/>
       <c r="H33" s="58"/>
       <c r="I33" s="58"/>
       <c r="J33" s="58"/>
       <c r="K33" s="58" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="L33" s="57" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M33" s="58"/>
       <c r="N33" s="58"/>
@@ -34945,17 +34982,17 @@
       <c r="D34" s="58"/>
       <c r="E34" s="58"/>
       <c r="F34" s="57" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="G34" s="58"/>
       <c r="H34" s="58"/>
       <c r="I34" s="58"/>
       <c r="J34" s="58"/>
       <c r="K34" s="58" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="L34" s="57" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="M34" s="58"/>
       <c r="N34" s="58"/>
@@ -34979,17 +35016,17 @@
       <c r="D35" s="58"/>
       <c r="E35" s="58"/>
       <c r="F35" s="57" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="G35" s="58"/>
       <c r="H35" s="58"/>
       <c r="I35" s="58"/>
       <c r="J35" s="58"/>
       <c r="K35" s="58" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="L35" s="57" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="M35" s="58"/>
       <c r="N35" s="58"/>
@@ -35013,17 +35050,17 @@
       <c r="D36" s="58"/>
       <c r="E36" s="58"/>
       <c r="F36" s="57" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="G36" s="58"/>
       <c r="H36" s="58"/>
       <c r="I36" s="58"/>
       <c r="J36" s="58"/>
       <c r="K36" s="58" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="L36" s="57" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="M36" s="58"/>
       <c r="N36" s="58"/>
@@ -35047,17 +35084,17 @@
       <c r="D37" s="58"/>
       <c r="E37" s="58"/>
       <c r="F37" s="57" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="G37" s="58"/>
       <c r="H37" s="58"/>
       <c r="I37" s="58"/>
       <c r="J37" s="58"/>
       <c r="K37" s="58" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="L37" s="57" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="M37" s="58"/>
       <c r="N37" s="58"/>
@@ -35081,17 +35118,17 @@
       <c r="D38" s="58"/>
       <c r="E38" s="58"/>
       <c r="F38" s="57" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="G38" s="58"/>
       <c r="H38" s="58"/>
       <c r="I38" s="58"/>
       <c r="J38" s="58"/>
       <c r="K38" s="58" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="L38" s="57" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="M38" s="58"/>
       <c r="N38" s="58"/>
@@ -35115,17 +35152,17 @@
       <c r="D39" s="58"/>
       <c r="E39" s="58"/>
       <c r="F39" s="57" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="G39" s="58"/>
       <c r="H39" s="58"/>
       <c r="I39" s="58"/>
       <c r="J39" s="58"/>
       <c r="K39" s="58" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="L39" s="57" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="M39" s="58"/>
       <c r="N39" s="58"/>
@@ -35149,17 +35186,17 @@
       <c r="D40" s="58"/>
       <c r="E40" s="58"/>
       <c r="F40" s="57" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G40" s="58"/>
       <c r="H40" s="58"/>
       <c r="I40" s="58"/>
       <c r="J40" s="58"/>
       <c r="K40" s="58" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="L40" s="57" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="M40" s="58"/>
       <c r="N40" s="58"/>
@@ -35183,17 +35220,17 @@
       <c r="D41" s="58"/>
       <c r="E41" s="58"/>
       <c r="F41" s="57" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="G41" s="58"/>
       <c r="H41" s="58"/>
       <c r="I41" s="58"/>
       <c r="J41" s="58"/>
       <c r="K41" s="58" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="L41" s="57" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="M41" s="58"/>
       <c r="N41" s="58"/>
@@ -35217,17 +35254,17 @@
       <c r="D42" s="58"/>
       <c r="E42" s="58"/>
       <c r="F42" s="57" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="G42" s="58"/>
       <c r="H42" s="58"/>
       <c r="I42" s="58"/>
       <c r="J42" s="58"/>
       <c r="K42" s="58" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="L42" s="57" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="M42" s="58"/>
       <c r="N42" s="58"/>
@@ -35251,17 +35288,17 @@
       <c r="D43" s="58"/>
       <c r="E43" s="58"/>
       <c r="F43" s="57" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="G43" s="58"/>
       <c r="H43" s="58"/>
       <c r="I43" s="58"/>
       <c r="J43" s="58"/>
       <c r="K43" s="58" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="L43" s="57" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="M43" s="58"/>
       <c r="N43" s="58"/>
@@ -35285,17 +35322,17 @@
       <c r="D44" s="58"/>
       <c r="E44" s="58"/>
       <c r="F44" s="57" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="G44" s="58"/>
       <c r="H44" s="58"/>
       <c r="I44" s="58"/>
       <c r="J44" s="58"/>
       <c r="K44" s="58" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="L44" s="57" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="M44" s="58"/>
       <c r="N44" s="58"/>
@@ -35319,14 +35356,14 @@
       <c r="D45" s="58"/>
       <c r="E45" s="58"/>
       <c r="F45" s="57" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="G45" s="58"/>
       <c r="H45" s="58"/>
       <c r="I45" s="58"/>
       <c r="J45" s="58"/>
       <c r="K45" s="58" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="L45" s="58"/>
       <c r="M45" s="58"/>
@@ -35351,14 +35388,14 @@
       <c r="D46" s="58"/>
       <c r="E46" s="58"/>
       <c r="F46" s="57" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="G46" s="58"/>
       <c r="H46" s="58"/>
       <c r="I46" s="58"/>
       <c r="J46" s="58"/>
       <c r="K46" s="58" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="L46" s="58"/>
       <c r="M46" s="58"/>
@@ -35383,14 +35420,14 @@
       <c r="D47" s="58"/>
       <c r="E47" s="58"/>
       <c r="F47" s="57" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="G47" s="58"/>
       <c r="H47" s="58"/>
       <c r="I47" s="58"/>
       <c r="J47" s="58"/>
       <c r="K47" s="58" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="L47" s="58"/>
       <c r="M47" s="58"/>
@@ -35415,14 +35452,14 @@
       <c r="D48" s="58"/>
       <c r="E48" s="58"/>
       <c r="F48" s="57" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="G48" s="58"/>
       <c r="H48" s="58"/>
       <c r="I48" s="58"/>
       <c r="J48" s="58"/>
       <c r="K48" s="58" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="L48" s="58"/>
       <c r="M48" s="58"/>
@@ -35447,14 +35484,14 @@
       <c r="D49" s="58"/>
       <c r="E49" s="58"/>
       <c r="F49" s="57" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G49" s="58"/>
       <c r="H49" s="58"/>
       <c r="I49" s="58"/>
       <c r="J49" s="58"/>
       <c r="K49" s="58" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="L49" s="58"/>
       <c r="M49" s="58"/>
@@ -35479,14 +35516,14 @@
       <c r="D50" s="58"/>
       <c r="E50" s="58"/>
       <c r="F50" s="57" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G50" s="58"/>
       <c r="H50" s="58"/>
       <c r="I50" s="58"/>
       <c r="J50" s="58"/>
       <c r="K50" s="58" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="L50" s="58"/>
       <c r="M50" s="58"/>
@@ -35511,14 +35548,14 @@
       <c r="D51" s="58"/>
       <c r="E51" s="58"/>
       <c r="F51" s="57" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="G51" s="58"/>
       <c r="H51" s="58"/>
       <c r="I51" s="58"/>
       <c r="J51" s="58"/>
       <c r="K51" s="58" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="L51" s="58"/>
       <c r="M51" s="58"/>
@@ -35543,14 +35580,14 @@
       <c r="D52" s="58"/>
       <c r="E52" s="58"/>
       <c r="F52" s="57" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="G52" s="58"/>
       <c r="H52" s="58"/>
       <c r="I52" s="58"/>
       <c r="J52" s="58"/>
       <c r="K52" s="58" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="L52" s="58"/>
       <c r="M52" s="58"/>
@@ -35575,14 +35612,14 @@
       <c r="D53" s="58"/>
       <c r="E53" s="58"/>
       <c r="F53" s="57" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="G53" s="58"/>
       <c r="H53" s="58"/>
       <c r="I53" s="58"/>
       <c r="J53" s="58"/>
       <c r="K53" s="58" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="L53" s="58"/>
       <c r="M53" s="58"/>
@@ -35607,14 +35644,14 @@
       <c r="D54" s="58"/>
       <c r="E54" s="58"/>
       <c r="F54" s="57" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="G54" s="58"/>
       <c r="H54" s="58"/>
       <c r="I54" s="58"/>
       <c r="J54" s="58"/>
       <c r="K54" s="58" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="L54" s="58"/>
       <c r="M54" s="58"/>
@@ -35639,14 +35676,14 @@
       <c r="D55" s="58"/>
       <c r="E55" s="58"/>
       <c r="F55" s="57" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="G55" s="58"/>
       <c r="H55" s="58"/>
       <c r="I55" s="58"/>
       <c r="J55" s="58"/>
       <c r="K55" s="58" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="L55" s="58"/>
       <c r="M55" s="58"/>
@@ -35671,14 +35708,14 @@
       <c r="D56" s="58"/>
       <c r="E56" s="58"/>
       <c r="F56" s="57" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G56" s="58"/>
       <c r="H56" s="58"/>
       <c r="I56" s="58"/>
       <c r="J56" s="58"/>
       <c r="K56" s="58" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="L56" s="58"/>
       <c r="M56" s="58"/>
@@ -35703,14 +35740,14 @@
       <c r="D57" s="58"/>
       <c r="E57" s="58"/>
       <c r="F57" s="57" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G57" s="58"/>
       <c r="H57" s="58"/>
       <c r="I57" s="58"/>
       <c r="J57" s="58"/>
       <c r="K57" s="58" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="L57" s="58"/>
       <c r="M57" s="58"/>
@@ -35735,14 +35772,14 @@
       <c r="D58" s="58"/>
       <c r="E58" s="58"/>
       <c r="F58" s="57" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="G58" s="58"/>
       <c r="H58" s="58"/>
       <c r="I58" s="58"/>
       <c r="J58" s="58"/>
       <c r="K58" s="58" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="L58" s="58"/>
       <c r="M58" s="58"/>
@@ -35767,14 +35804,14 @@
       <c r="D59" s="58"/>
       <c r="E59" s="58"/>
       <c r="F59" s="57" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="G59" s="58"/>
       <c r="H59" s="58"/>
       <c r="I59" s="58"/>
       <c r="J59" s="58"/>
       <c r="K59" s="58" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="L59" s="58"/>
       <c r="M59" s="58"/>
@@ -35799,14 +35836,14 @@
       <c r="D60" s="58"/>
       <c r="E60" s="58"/>
       <c r="F60" s="57" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="G60" s="58"/>
       <c r="H60" s="58"/>
       <c r="I60" s="58"/>
       <c r="J60" s="58"/>
       <c r="K60" s="58" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="L60" s="58"/>
       <c r="M60" s="58"/>
@@ -35831,14 +35868,14 @@
       <c r="D61" s="58"/>
       <c r="E61" s="58"/>
       <c r="F61" s="57" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="G61" s="58"/>
       <c r="H61" s="58"/>
       <c r="I61" s="58"/>
       <c r="J61" s="58"/>
       <c r="K61" s="58" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="L61" s="58"/>
       <c r="M61" s="58"/>
@@ -35863,14 +35900,14 @@
       <c r="D62" s="58"/>
       <c r="E62" s="58"/>
       <c r="F62" s="57" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="G62" s="58"/>
       <c r="H62" s="58"/>
       <c r="I62" s="58"/>
       <c r="J62" s="58"/>
       <c r="K62" s="58" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="L62" s="58"/>
       <c r="M62" s="58"/>
@@ -35895,14 +35932,14 @@
       <c r="D63" s="58"/>
       <c r="E63" s="58"/>
       <c r="F63" s="57" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="G63" s="58"/>
       <c r="H63" s="58"/>
       <c r="I63" s="58"/>
       <c r="J63" s="58"/>
       <c r="K63" s="58" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="L63" s="58"/>
       <c r="M63" s="58"/>
@@ -35927,14 +35964,14 @@
       <c r="D64" s="58"/>
       <c r="E64" s="58"/>
       <c r="F64" s="57" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="G64" s="58"/>
       <c r="H64" s="58"/>
       <c r="I64" s="58"/>
       <c r="J64" s="58"/>
       <c r="K64" s="58" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="L64" s="58"/>
       <c r="M64" s="58"/>
@@ -35959,14 +35996,14 @@
       <c r="D65" s="58"/>
       <c r="E65" s="58"/>
       <c r="F65" s="57" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="G65" s="58"/>
       <c r="H65" s="58"/>
       <c r="I65" s="58"/>
       <c r="J65" s="58"/>
       <c r="K65" s="58" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="L65" s="58"/>
       <c r="M65" s="58"/>
@@ -35991,14 +36028,14 @@
       <c r="D66" s="58"/>
       <c r="E66" s="58"/>
       <c r="F66" s="57" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="G66" s="58"/>
       <c r="H66" s="58"/>
       <c r="I66" s="58"/>
       <c r="J66" s="58"/>
       <c r="K66" s="58" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="L66" s="58"/>
       <c r="M66" s="58"/>
@@ -36023,14 +36060,14 @@
       <c r="D67" s="58"/>
       <c r="E67" s="58"/>
       <c r="F67" s="57" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="G67" s="58"/>
       <c r="H67" s="58"/>
       <c r="I67" s="58"/>
       <c r="J67" s="58"/>
       <c r="K67" s="58" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="L67" s="58"/>
       <c r="M67" s="58"/>
@@ -36055,14 +36092,14 @@
       <c r="D68" s="58"/>
       <c r="E68" s="58"/>
       <c r="F68" s="57" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="G68" s="58"/>
       <c r="H68" s="58"/>
       <c r="I68" s="58"/>
       <c r="J68" s="58"/>
       <c r="K68" s="58" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="L68" s="58"/>
       <c r="M68" s="58"/>
@@ -36087,14 +36124,14 @@
       <c r="D69" s="58"/>
       <c r="E69" s="58"/>
       <c r="F69" s="57" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="G69" s="58"/>
       <c r="H69" s="58"/>
       <c r="I69" s="58"/>
       <c r="J69" s="58"/>
       <c r="K69" s="58" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="L69" s="58"/>
       <c r="M69" s="58"/>
@@ -36119,14 +36156,14 @@
       <c r="D70" s="58"/>
       <c r="E70" s="58"/>
       <c r="F70" s="57" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="G70" s="58"/>
       <c r="H70" s="58"/>
       <c r="I70" s="58"/>
       <c r="J70" s="58"/>
       <c r="K70" s="58" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="L70" s="58"/>
       <c r="M70" s="58"/>
@@ -36151,14 +36188,14 @@
       <c r="D71" s="58"/>
       <c r="E71" s="58"/>
       <c r="F71" s="57" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G71" s="58"/>
       <c r="H71" s="58"/>
       <c r="I71" s="58"/>
       <c r="J71" s="58"/>
       <c r="K71" s="58" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="L71" s="58"/>
       <c r="M71" s="58"/>
@@ -36183,14 +36220,14 @@
       <c r="D72" s="58"/>
       <c r="E72" s="58"/>
       <c r="F72" s="57" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="G72" s="58"/>
       <c r="H72" s="58"/>
       <c r="I72" s="58"/>
       <c r="J72" s="58"/>
       <c r="K72" s="58" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="L72" s="58"/>
       <c r="M72" s="58"/>
@@ -36215,14 +36252,14 @@
       <c r="D73" s="58"/>
       <c r="E73" s="58"/>
       <c r="F73" s="57" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="G73" s="58"/>
       <c r="H73" s="58"/>
       <c r="I73" s="58"/>
       <c r="J73" s="58"/>
       <c r="K73" s="58" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="L73" s="58"/>
       <c r="M73" s="58"/>
@@ -36247,14 +36284,14 @@
       <c r="D74" s="58"/>
       <c r="E74" s="58"/>
       <c r="F74" s="57" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="G74" s="58"/>
       <c r="H74" s="58"/>
       <c r="I74" s="58"/>
       <c r="J74" s="58"/>
       <c r="K74" s="58" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="L74" s="58"/>
       <c r="M74" s="58"/>
@@ -36279,14 +36316,14 @@
       <c r="D75" s="58"/>
       <c r="E75" s="58"/>
       <c r="F75" s="57" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="G75" s="58"/>
       <c r="H75" s="58"/>
       <c r="I75" s="58"/>
       <c r="J75" s="58"/>
       <c r="K75" s="58" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="L75" s="58"/>
       <c r="M75" s="58"/>
@@ -36311,14 +36348,14 @@
       <c r="D76" s="58"/>
       <c r="E76" s="58"/>
       <c r="F76" s="57" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="G76" s="58"/>
       <c r="H76" s="58"/>
       <c r="I76" s="58"/>
       <c r="J76" s="58"/>
       <c r="K76" s="58" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="L76" s="58"/>
       <c r="M76" s="58"/>
@@ -36343,14 +36380,14 @@
       <c r="D77" s="58"/>
       <c r="E77" s="58"/>
       <c r="F77" s="57" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="G77" s="58"/>
       <c r="H77" s="58"/>
       <c r="I77" s="58"/>
       <c r="J77" s="58"/>
       <c r="K77" s="58" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="L77" s="58"/>
       <c r="M77" s="58"/>
@@ -36375,7 +36412,7 @@
       <c r="D78" s="58"/>
       <c r="E78" s="58"/>
       <c r="F78" s="57" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="G78" s="58"/>
       <c r="H78" s="58"/>
@@ -36405,7 +36442,7 @@
       <c r="D79" s="58"/>
       <c r="E79" s="58"/>
       <c r="F79" s="57" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="G79" s="58"/>
       <c r="H79" s="58"/>
@@ -36435,7 +36472,7 @@
       <c r="D80" s="58"/>
       <c r="E80" s="58"/>
       <c r="F80" s="57" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="G80" s="58"/>
       <c r="H80" s="58"/>
@@ -36465,7 +36502,7 @@
       <c r="D81" s="58"/>
       <c r="E81" s="58"/>
       <c r="F81" s="57" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="G81" s="58"/>
       <c r="H81" s="58"/>
@@ -36495,7 +36532,7 @@
       <c r="D82" s="58"/>
       <c r="E82" s="58"/>
       <c r="F82" s="57" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G82" s="58"/>
       <c r="H82" s="58"/>
@@ -36525,7 +36562,7 @@
       <c r="D83" s="58"/>
       <c r="E83" s="58"/>
       <c r="F83" s="57" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="G83" s="58"/>
       <c r="H83" s="58"/>
@@ -36555,7 +36592,7 @@
       <c r="D84" s="58"/>
       <c r="E84" s="58"/>
       <c r="F84" s="57" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G84" s="58"/>
       <c r="H84" s="58"/>
@@ -36585,7 +36622,7 @@
       <c r="D85" s="58"/>
       <c r="E85" s="58"/>
       <c r="F85" s="57" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="G85" s="58"/>
       <c r="H85" s="58"/>
@@ -36615,7 +36652,7 @@
       <c r="D86" s="58"/>
       <c r="E86" s="58"/>
       <c r="F86" s="57" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="G86" s="58"/>
       <c r="H86" s="58"/>
@@ -36645,7 +36682,7 @@
       <c r="D87" s="58"/>
       <c r="E87" s="58"/>
       <c r="F87" s="57" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="G87" s="58"/>
       <c r="H87" s="58"/>
@@ -36675,7 +36712,7 @@
       <c r="D88" s="58"/>
       <c r="E88" s="58"/>
       <c r="F88" s="57" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="G88" s="58"/>
       <c r="H88" s="58"/>
@@ -36705,7 +36742,7 @@
       <c r="D89" s="58"/>
       <c r="E89" s="58"/>
       <c r="F89" s="57" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="G89" s="58"/>
       <c r="H89" s="58"/>
@@ -36735,7 +36772,7 @@
       <c r="D90" s="58"/>
       <c r="E90" s="58"/>
       <c r="F90" s="57" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="G90" s="58"/>
       <c r="H90" s="58"/>
@@ -36765,7 +36802,7 @@
       <c r="D91" s="58"/>
       <c r="E91" s="58"/>
       <c r="F91" s="57" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="G91" s="58"/>
       <c r="H91" s="58"/>
@@ -36795,7 +36832,7 @@
       <c r="D92" s="58"/>
       <c r="E92" s="58"/>
       <c r="F92" s="57" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="G92" s="58"/>
       <c r="H92" s="58"/>
@@ -36825,7 +36862,7 @@
       <c r="D93" s="58"/>
       <c r="E93" s="58"/>
       <c r="F93" s="57" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="G93" s="58"/>
       <c r="H93" s="58"/>

</xml_diff>

<commit_message>
Don't set `idno` for storage locations
* Update view for storage locations
</commit_message>
<xml_diff>
--- a/museum/rwahsLocationHistoryMapping.xlsx
+++ b/museum/rwahsLocationHistoryMapping.xlsx
@@ -310,7 +310,7 @@
     "storageLocationType": "^childType",
     "relationshipType": "related",
     "attributes":{
-        "idno": "%",
+        "idno": "",
         "is_enabled": true,
         "status": "completed"
     },
@@ -321,7 +321,7 @@
         {
             "name": "^topLevelLocation",
             "type": "room",
-            "idno": "%",
+            "idno": "",
             "attributes":{
                 "is_enabled": true
             }

</xml_diff>

<commit_message>
Update location history sample data to include objects which have more than a single location record
</commit_message>
<xml_diff>
--- a/museum/rwahsLocationHistoryMapping.xlsx
+++ b/museum/rwahsLocationHistoryMapping.xlsx
@@ -2242,7 +2242,7 @@
       <c r="L16" s="31"/>
       <c r="M16" s="32" t="str">
         <f t="shared" ref="M16:M18" si="1">validateJson(E16, G16)</f>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N16" s="33"/>
       <c r="O16" s="33" t="s">
@@ -2340,7 +2340,7 @@
       <c r="L17" s="31"/>
       <c r="M17" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N17" s="33" t="s">
         <v>68</v>
@@ -2430,7 +2430,7 @@
       <c r="L18" s="31"/>
       <c r="M18" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N18" s="33"/>
       <c r="O18" s="33" t="s">
@@ -2595,7 +2595,7 @@
       <c r="L20" s="31"/>
       <c r="M20" s="32" t="str">
         <f>validateJson(E20, G20)</f>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N20" s="33" t="s">
         <v>68</v>
@@ -2889,7 +2889,7 @@
       <c r="L24" s="31"/>
       <c r="M24" s="32" t="str">
         <f t="shared" ref="M24:M25" si="12">validateJson(E24, G24)</f>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N24" s="33"/>
       <c r="O24" s="33" t="s">
@@ -2973,7 +2973,7 @@
       <c r="L25" s="31"/>
       <c r="M25" s="32" t="str">
         <f t="shared" si="12"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N25" s="33"/>
       <c r="O25" s="33" t="s">
@@ -3256,7 +3256,7 @@
       <c r="L29" s="31"/>
       <c r="M29" s="32" t="str">
         <f t="shared" ref="M29:M30" si="13">validateJson(E29, G29)</f>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N29" s="34"/>
       <c r="O29" s="34"/>
@@ -3338,7 +3338,7 @@
       <c r="L30" s="31"/>
       <c r="M30" s="32" t="str">
         <f t="shared" si="13"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N30" s="34"/>
       <c r="O30" s="34"/>
@@ -3450,7 +3450,7 @@
       </c>
       <c r="Y31" s="34" t="str">
         <f t="shared" ref="Y31:Y38" si="14">camelToTitle(X31)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z31" s="33" t="s">
         <v>95</v>
@@ -3463,17 +3463,7 @@
       <c r="AD31" s="34"/>
       <c r="AE31" s="35" t="str">
         <f t="shared" si="11"/>
-        <v>&lt;metadataElement code='' datatype='Text'&gt;
-  &lt;labels&gt;&lt;label locale='en_AU'&gt;&lt;name&gt;&lt;/name&gt;&lt;/label&gt;&lt;/labels&gt;
-  &lt;typeRestrictions&gt;
-    &lt;restriction code='museum_'&gt;
-       &lt;table&gt;&lt;/table&gt;
-       &lt;type&gt;museum&lt;/type&gt;
-       &lt;includeSubtypes&gt;true&lt;/includeSubtypes&gt;
-    &lt;/restriction&gt;
-  &lt;/typeRestrictions&gt;
-&lt;/metadataElement&gt;
-</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="32">
@@ -3493,7 +3483,7 @@
       <c r="L32" s="31"/>
       <c r="M32" s="32" t="str">
         <f t="shared" ref="M32:M38" si="15">validateJson(E32, G32)</f>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N32" s="33"/>
       <c r="O32" s="33" t="s">
@@ -3537,7 +3527,7 @@
       </c>
       <c r="Y32" s="34" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z32" s="33" t="s">
         <v>95</v>
@@ -3554,17 +3544,7 @@
       </c>
       <c r="AE32" s="35" t="str">
         <f t="shared" si="11"/>
-        <v>&lt;metadataElement code='' datatype='Text'&gt;
-  &lt;labels&gt;&lt;label locale='en_AU'&gt;&lt;name&gt;&lt;/name&gt;&lt;/label&gt;&lt;/labels&gt;
-  &lt;typeRestrictions&gt;
-    &lt;restriction code='museum_'&gt;
-       &lt;table&gt;&lt;/table&gt;
-       &lt;type&gt;museum&lt;/type&gt;
-       &lt;includeSubtypes&gt;true&lt;/includeSubtypes&gt;
-    &lt;/restriction&gt;
-  &lt;/typeRestrictions&gt;
-&lt;/metadataElement&gt;
-</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="33">
@@ -3584,7 +3564,7 @@
       <c r="L33" s="31"/>
       <c r="M33" s="32" t="str">
         <f t="shared" si="15"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N33" s="33"/>
       <c r="O33" s="33" t="s">
@@ -3628,7 +3608,7 @@
       </c>
       <c r="Y33" s="34" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z33" s="33" t="s">
         <v>95</v>
@@ -3645,17 +3625,7 @@
       </c>
       <c r="AE33" s="35" t="str">
         <f t="shared" si="11"/>
-        <v>&lt;metadataElement code='' datatype='Text'&gt;
-  &lt;labels&gt;&lt;label locale='en_AU'&gt;&lt;name&gt;&lt;/name&gt;&lt;/label&gt;&lt;/labels&gt;
-  &lt;typeRestrictions&gt;
-    &lt;restriction code='museum_'&gt;
-       &lt;table&gt;&lt;/table&gt;
-       &lt;type&gt;museum&lt;/type&gt;
-       &lt;includeSubtypes&gt;true&lt;/includeSubtypes&gt;
-    &lt;/restriction&gt;
-  &lt;/typeRestrictions&gt;
-&lt;/metadataElement&gt;
-</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="34">
@@ -3675,7 +3645,7 @@
       <c r="L34" s="31"/>
       <c r="M34" s="32" t="str">
         <f t="shared" si="15"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N34" s="33"/>
       <c r="O34" s="33" t="s">
@@ -3704,7 +3674,7 @@
       </c>
       <c r="Y34" s="34" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z34" s="33" t="s">
         <v>97</v>
@@ -3715,17 +3685,7 @@
       <c r="AD34" s="34"/>
       <c r="AE34" s="35" t="str">
         <f t="shared" si="11"/>
-        <v>&lt;metadataElement code='' datatype='DateRange'&gt;
-  &lt;labels&gt;&lt;label locale='en_AU'&gt;&lt;name&gt;&lt;/name&gt;&lt;/label&gt;&lt;/labels&gt;
-  &lt;typeRestrictions&gt;
-    &lt;restriction code='museum_'&gt;
-       &lt;table&gt;&lt;/table&gt;
-       &lt;type&gt;museum&lt;/type&gt;
-       &lt;includeSubtypes&gt;true&lt;/includeSubtypes&gt;
-    &lt;/restriction&gt;
-  &lt;/typeRestrictions&gt;
-&lt;/metadataElement&gt;
-</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="35">
@@ -3745,7 +3705,7 @@
       <c r="L35" s="31"/>
       <c r="M35" s="32" t="str">
         <f t="shared" si="15"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N35" s="33"/>
       <c r="O35" s="33" t="s">
@@ -3789,7 +3749,7 @@
       </c>
       <c r="Y35" s="34" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z35" s="33" t="s">
         <v>97</v>
@@ -3806,17 +3766,7 @@
       </c>
       <c r="AE35" s="35" t="str">
         <f t="shared" si="11"/>
-        <v>&lt;metadataElement code='' datatype='DateRange'&gt;
-  &lt;labels&gt;&lt;label locale='en_AU'&gt;&lt;name&gt;&lt;/name&gt;&lt;/label&gt;&lt;/labels&gt;
-  &lt;typeRestrictions&gt;
-    &lt;restriction code='museum_'&gt;
-       &lt;table&gt;&lt;/table&gt;
-       &lt;type&gt;museum&lt;/type&gt;
-       &lt;includeSubtypes&gt;true&lt;/includeSubtypes&gt;
-    &lt;/restriction&gt;
-  &lt;/typeRestrictions&gt;
-&lt;/metadataElement&gt;
-</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="36">
@@ -3836,7 +3786,7 @@
       <c r="L36" s="31"/>
       <c r="M36" s="32" t="str">
         <f t="shared" si="15"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N36" s="33"/>
       <c r="O36" s="33" t="s">
@@ -3865,7 +3815,7 @@
       </c>
       <c r="Y36" s="34" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z36" s="33" t="s">
         <v>95</v>
@@ -3876,17 +3826,7 @@
       <c r="AD36" s="34"/>
       <c r="AE36" s="35" t="str">
         <f t="shared" si="11"/>
-        <v>&lt;metadataElement code='' datatype='Text'&gt;
-  &lt;labels&gt;&lt;label locale='en_AU'&gt;&lt;name&gt;&lt;/name&gt;&lt;/label&gt;&lt;/labels&gt;
-  &lt;typeRestrictions&gt;
-    &lt;restriction code='museum_'&gt;
-       &lt;table&gt;&lt;/table&gt;
-       &lt;type&gt;museum&lt;/type&gt;
-       &lt;includeSubtypes&gt;true&lt;/includeSubtypes&gt;
-    &lt;/restriction&gt;
-  &lt;/typeRestrictions&gt;
-&lt;/metadataElement&gt;
-</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="37">
@@ -3906,7 +3846,7 @@
       <c r="L37" s="31"/>
       <c r="M37" s="32" t="str">
         <f t="shared" si="15"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N37" s="33"/>
       <c r="O37" s="33" t="s">
@@ -3950,7 +3890,7 @@
       </c>
       <c r="Y37" s="34" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z37" s="33" t="s">
         <v>98</v>
@@ -3967,17 +3907,7 @@
       </c>
       <c r="AE37" s="35" t="str">
         <f t="shared" si="11"/>
-        <v>&lt;metadataElement code='' datatype='Entities'&gt;
-  &lt;labels&gt;&lt;label locale='en_AU'&gt;&lt;name&gt;&lt;/name&gt;&lt;/label&gt;&lt;/labels&gt;
-  &lt;typeRestrictions&gt;
-    &lt;restriction code='museum_'&gt;
-       &lt;table&gt;&lt;/table&gt;
-       &lt;type&gt;museum&lt;/type&gt;
-       &lt;includeSubtypes&gt;true&lt;/includeSubtypes&gt;
-    &lt;/restriction&gt;
-  &lt;/typeRestrictions&gt;
-&lt;/metadataElement&gt;
-</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="38">
@@ -3997,7 +3927,7 @@
       <c r="L38" s="31"/>
       <c r="M38" s="32" t="str">
         <f t="shared" si="15"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N38" s="33"/>
       <c r="O38" s="33" t="s">
@@ -4026,7 +3956,7 @@
       </c>
       <c r="Y38" s="34" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z38" s="33" t="s">
         <v>95</v>
@@ -4039,17 +3969,7 @@
       <c r="AD38" s="34"/>
       <c r="AE38" s="35" t="str">
         <f t="shared" si="11"/>
-        <v>&lt;metadataElement code='' datatype='Text'&gt;
-  &lt;labels&gt;&lt;label locale='en_AU'&gt;&lt;name&gt;&lt;/name&gt;&lt;/label&gt;&lt;/labels&gt;
-  &lt;typeRestrictions&gt;
-    &lt;restriction code='museum_'&gt;
-       &lt;table&gt;&lt;/table&gt;
-       &lt;type&gt;museum&lt;/type&gt;
-       &lt;includeSubtypes&gt;true&lt;/includeSubtypes&gt;
-    &lt;/restriction&gt;
-  &lt;/typeRestrictions&gt;
-&lt;/metadataElement&gt;
-</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="39">
@@ -4377,7 +4297,7 @@
       <c r="L44" s="31"/>
       <c r="M44" s="32" t="str">
         <f t="shared" ref="M44:M58" si="20">validateJson(E44, G44)</f>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N44" s="33"/>
       <c r="O44" s="33" t="s">
@@ -4421,7 +4341,7 @@
       </c>
       <c r="Y44" s="34" t="str">
         <f t="shared" ref="Y44:Y59" si="21">camelToTitle(X44)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z44" s="33" t="s">
         <v>20</v>
@@ -4470,7 +4390,7 @@
       <c r="L45" s="31"/>
       <c r="M45" s="32" t="str">
         <f t="shared" si="20"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N45" s="33"/>
       <c r="O45" s="33" t="s">
@@ -4514,7 +4434,7 @@
       </c>
       <c r="Y45" s="34" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z45" s="33" t="s">
         <v>20</v>
@@ -4553,7 +4473,7 @@
       <c r="L46" s="31"/>
       <c r="M46" s="32" t="str">
         <f t="shared" si="20"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N46" s="33"/>
       <c r="O46" s="33" t="s">
@@ -4597,7 +4517,7 @@
       </c>
       <c r="Y46" s="34" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z46" s="33" t="s">
         <v>20</v>
@@ -4636,7 +4556,7 @@
       <c r="L47" s="31"/>
       <c r="M47" s="32" t="str">
         <f t="shared" si="20"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N47" s="33"/>
       <c r="O47" s="33" t="s">
@@ -4680,7 +4600,7 @@
       </c>
       <c r="Y47" s="34" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z47" s="33" t="s">
         <v>20</v>
@@ -4719,7 +4639,7 @@
       <c r="L48" s="31"/>
       <c r="M48" s="32" t="str">
         <f t="shared" si="20"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N48" s="33"/>
       <c r="O48" s="33" t="s">
@@ -4763,7 +4683,7 @@
       </c>
       <c r="Y48" s="34" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z48" s="33" t="s">
         <v>20</v>
@@ -4802,7 +4722,7 @@
       <c r="L49" s="31"/>
       <c r="M49" s="32" t="str">
         <f t="shared" si="20"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N49" s="33"/>
       <c r="O49" s="33" t="s">
@@ -4846,7 +4766,7 @@
       </c>
       <c r="Y49" s="34" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z49" s="33" t="s">
         <v>20</v>
@@ -4885,7 +4805,7 @@
       <c r="L50" s="31"/>
       <c r="M50" s="32" t="str">
         <f t="shared" si="20"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N50" s="33"/>
       <c r="O50" s="33" t="s">
@@ -4914,7 +4834,7 @@
       </c>
       <c r="Y50" s="34" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z50" s="33" t="s">
         <v>20</v>
@@ -4947,7 +4867,7 @@
       <c r="L51" s="31"/>
       <c r="M51" s="32" t="str">
         <f t="shared" si="20"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N51" s="33"/>
       <c r="O51" s="33" t="s">
@@ -4976,7 +4896,7 @@
       </c>
       <c r="Y51" s="34" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z51" s="33" t="s">
         <v>20</v>
@@ -5009,7 +4929,7 @@
       <c r="L52" s="31"/>
       <c r="M52" s="32" t="str">
         <f t="shared" si="20"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N52" s="33"/>
       <c r="O52" s="33" t="s">
@@ -5053,7 +4973,7 @@
       </c>
       <c r="Y52" s="34" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z52" s="33" t="s">
         <v>20</v>
@@ -5092,7 +5012,7 @@
       <c r="L53" s="31"/>
       <c r="M53" s="32" t="str">
         <f t="shared" si="20"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N53" s="33"/>
       <c r="O53" s="33" t="s">
@@ -5136,7 +5056,7 @@
       </c>
       <c r="Y53" s="34" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z53" s="33" t="s">
         <v>20</v>
@@ -5175,7 +5095,7 @@
       <c r="L54" s="31"/>
       <c r="M54" s="32" t="str">
         <f t="shared" si="20"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N54" s="33"/>
       <c r="O54" s="33" t="s">
@@ -5219,7 +5139,7 @@
       </c>
       <c r="Y54" s="34" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z54" s="33" t="s">
         <v>20</v>
@@ -5258,7 +5178,7 @@
       <c r="L55" s="31"/>
       <c r="M55" s="32" t="str">
         <f t="shared" si="20"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N55" s="33"/>
       <c r="O55" s="33" t="s">
@@ -5302,7 +5222,7 @@
       </c>
       <c r="Y55" s="34" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z55" s="33" t="s">
         <v>20</v>
@@ -5341,7 +5261,7 @@
       <c r="L56" s="31"/>
       <c r="M56" s="32" t="str">
         <f t="shared" si="20"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N56" s="33"/>
       <c r="O56" s="33" t="s">
@@ -5385,7 +5305,7 @@
       </c>
       <c r="Y56" s="34" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z56" s="33" t="s">
         <v>20</v>
@@ -5424,7 +5344,7 @@
       <c r="L57" s="31"/>
       <c r="M57" s="32" t="str">
         <f t="shared" si="20"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N57" s="33"/>
       <c r="O57" s="33" t="s">
@@ -5468,7 +5388,7 @@
       </c>
       <c r="Y57" s="34" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z57" s="33" t="s">
         <v>95</v>
@@ -5505,7 +5425,7 @@
       <c r="L58" s="31"/>
       <c r="M58" s="32" t="str">
         <f t="shared" si="20"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N58" s="33"/>
       <c r="O58" s="33" t="s">
@@ -5549,7 +5469,7 @@
       </c>
       <c r="Y58" s="34" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z58" s="33" t="s">
         <v>95</v>
@@ -5612,7 +5532,7 @@
       </c>
       <c r="Y59" s="34" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z59" s="33" t="s">
         <v>95</v>
@@ -5781,7 +5701,7 @@
       <c r="L62" s="31"/>
       <c r="M62" s="32" t="str">
         <f t="shared" ref="M62:M73" si="25">validateJson(E62, G62)</f>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N62" s="34"/>
       <c r="O62" s="34"/>
@@ -5863,7 +5783,7 @@
       <c r="L63" s="31"/>
       <c r="M63" s="32" t="str">
         <f t="shared" si="25"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N63" s="34"/>
       <c r="O63" s="34"/>
@@ -5943,7 +5863,7 @@
       <c r="L64" s="31"/>
       <c r="M64" s="32" t="str">
         <f t="shared" si="25"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N64" s="34"/>
       <c r="O64" s="34"/>
@@ -6023,7 +5943,7 @@
       <c r="L65" s="31"/>
       <c r="M65" s="32" t="str">
         <f t="shared" si="25"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N65" s="34"/>
       <c r="O65" s="34"/>
@@ -6103,7 +6023,7 @@
       <c r="L66" s="31"/>
       <c r="M66" s="32" t="str">
         <f t="shared" si="25"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N66" s="34"/>
       <c r="O66" s="34"/>
@@ -6183,7 +6103,7 @@
       <c r="L67" s="31"/>
       <c r="M67" s="32" t="str">
         <f t="shared" si="25"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N67" s="34"/>
       <c r="O67" s="34"/>
@@ -6263,7 +6183,7 @@
       <c r="L68" s="31"/>
       <c r="M68" s="32" t="str">
         <f t="shared" si="25"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N68" s="34"/>
       <c r="O68" s="34"/>
@@ -6343,7 +6263,7 @@
       <c r="L69" s="31"/>
       <c r="M69" s="32" t="str">
         <f t="shared" si="25"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N69" s="34"/>
       <c r="O69" s="34"/>
@@ -6423,7 +6343,7 @@
       <c r="L70" s="31"/>
       <c r="M70" s="32" t="str">
         <f t="shared" si="25"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N70" s="34"/>
       <c r="O70" s="34"/>
@@ -6505,7 +6425,7 @@
       <c r="L71" s="31"/>
       <c r="M71" s="32" t="str">
         <f t="shared" si="25"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N71" s="34"/>
       <c r="O71" s="34"/>
@@ -6585,7 +6505,7 @@
       <c r="L72" s="31"/>
       <c r="M72" s="32" t="str">
         <f t="shared" si="25"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N72" s="34"/>
       <c r="O72" s="34"/>
@@ -6665,7 +6585,7 @@
       <c r="L73" s="45"/>
       <c r="M73" s="46" t="str">
         <f t="shared" si="25"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N73" s="47"/>
       <c r="O73" s="47"/>
@@ -6798,7 +6718,7 @@
       <c r="L75" s="31"/>
       <c r="M75" s="32" t="str">
         <f t="shared" ref="M75:M76" si="26">validateJson(E75, G75)</f>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N75" s="33"/>
       <c r="O75" s="33" t="s">
@@ -6842,7 +6762,7 @@
       </c>
       <c r="Y75" s="34" t="str">
         <f t="shared" ref="Y75:Y76" si="30">camelToTitle(X75)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z75" s="33" t="s">
         <v>20</v>
@@ -6891,7 +6811,7 @@
       <c r="L76" s="31"/>
       <c r="M76" s="32" t="str">
         <f t="shared" si="26"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N76" s="33"/>
       <c r="O76" s="33" t="s">
@@ -6935,7 +6855,7 @@
       </c>
       <c r="Y76" s="34" t="str">
         <f t="shared" si="30"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z76" s="33"/>
       <c r="AA76" s="33"/>
@@ -7043,7 +6963,7 @@
       <c r="L78" s="31"/>
       <c r="M78" s="32" t="str">
         <f t="shared" ref="M78:M86" si="34">validateJson(E78, G78)</f>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N78" s="34"/>
       <c r="O78" s="34"/>
@@ -7123,7 +7043,7 @@
       <c r="L79" s="31"/>
       <c r="M79" s="32" t="str">
         <f t="shared" si="34"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N79" s="34"/>
       <c r="O79" s="34"/>
@@ -7203,7 +7123,7 @@
       <c r="L80" s="31"/>
       <c r="M80" s="32" t="str">
         <f t="shared" si="34"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N80" s="34"/>
       <c r="O80" s="34"/>
@@ -7283,7 +7203,7 @@
       <c r="L81" s="31"/>
       <c r="M81" s="32" t="str">
         <f t="shared" si="34"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N81" s="33"/>
       <c r="O81" s="33" t="s">
@@ -7327,7 +7247,7 @@
       </c>
       <c r="Y81" s="34" t="str">
         <f t="shared" ref="Y81:Y83" si="35">camelToTitle(X81)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z81" s="33"/>
       <c r="AA81" s="33"/>
@@ -7372,7 +7292,7 @@
       <c r="L82" s="31"/>
       <c r="M82" s="32" t="str">
         <f t="shared" si="34"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N82" s="33"/>
       <c r="O82" s="33" t="s">
@@ -7416,7 +7336,7 @@
       </c>
       <c r="Y82" s="34" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z82" s="33"/>
       <c r="AA82" s="33"/>
@@ -7451,7 +7371,7 @@
       <c r="L83" s="31"/>
       <c r="M83" s="32" t="str">
         <f t="shared" si="34"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N83" s="34"/>
       <c r="O83" s="33"/>
@@ -7493,7 +7413,7 @@
       </c>
       <c r="Y83" s="34" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z83" s="33" t="s">
         <v>20</v>
@@ -7532,7 +7452,7 @@
       <c r="L84" s="31"/>
       <c r="M84" s="32" t="str">
         <f t="shared" si="34"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N84" s="34"/>
       <c r="O84" s="34"/>
@@ -7622,7 +7542,7 @@
       <c r="L85" s="31"/>
       <c r="M85" s="32" t="str">
         <f t="shared" si="34"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N85" s="34"/>
       <c r="O85" s="34"/>
@@ -7702,7 +7622,7 @@
       <c r="L86" s="31"/>
       <c r="M86" s="32" t="str">
         <f t="shared" si="34"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N86" s="34"/>
       <c r="O86" s="34"/>
@@ -7845,7 +7765,7 @@
       <c r="L88" s="31"/>
       <c r="M88" s="32" t="str">
         <f t="shared" ref="M88:M97" si="39">validateJson(E88, G88)</f>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N88" s="34"/>
       <c r="O88" s="34"/>
@@ -7925,7 +7845,7 @@
       <c r="L89" s="31"/>
       <c r="M89" s="32" t="str">
         <f t="shared" si="39"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N89" s="34"/>
       <c r="O89" s="34"/>
@@ -8005,7 +7925,7 @@
       <c r="L90" s="31"/>
       <c r="M90" s="32" t="str">
         <f t="shared" si="39"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N90" s="34"/>
       <c r="O90" s="34"/>
@@ -8085,7 +8005,7 @@
       <c r="L91" s="45"/>
       <c r="M91" s="46" t="str">
         <f t="shared" si="39"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N91" s="47"/>
       <c r="O91" s="47"/>
@@ -8165,7 +8085,7 @@
       <c r="L92" s="31"/>
       <c r="M92" s="32" t="str">
         <f t="shared" si="39"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N92" s="34"/>
       <c r="O92" s="34"/>
@@ -8245,7 +8165,7 @@
       <c r="L93" s="31"/>
       <c r="M93" s="32" t="str">
         <f t="shared" si="39"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N93" s="34"/>
       <c r="O93" s="34"/>
@@ -8325,7 +8245,7 @@
       <c r="L94" s="31"/>
       <c r="M94" s="32" t="str">
         <f t="shared" si="39"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N94" s="34"/>
       <c r="O94" s="34"/>
@@ -8405,7 +8325,7 @@
       <c r="L95" s="31"/>
       <c r="M95" s="32" t="str">
         <f t="shared" si="39"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N95" s="34"/>
       <c r="O95" s="34"/>
@@ -8485,7 +8405,7 @@
       <c r="L96" s="31"/>
       <c r="M96" s="32" t="str">
         <f t="shared" si="39"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N96" s="34"/>
       <c r="O96" s="34"/>
@@ -8565,7 +8485,7 @@
       <c r="L97" s="31"/>
       <c r="M97" s="32" t="str">
         <f t="shared" si="39"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N97" s="34"/>
       <c r="O97" s="34"/>

</xml_diff>